<commit_message>
Update the json sample
</commit_message>
<xml_diff>
--- a/LSCS-Tool-schema.xlsx
+++ b/LSCS-Tool-schema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Definition" sheetId="1" r:id="rId1"/>
@@ -304,8 +304,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>158750</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -315,7 +315,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="171450" y="57150"/>
-          <a:ext cx="4254500" cy="1790700"/>
+          <a:ext cx="4254500" cy="2857500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -359,7 +359,187 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>{ "@context": "http://schema.org", "@type": "SoftwareApplication", "name": "Primer3", "description": "The open-source software which is a widely used application for PCR primer design that includes more accurate thermodynamic models and the ability to use lowercase masked template sequences.", "softwareVersion": "1.0", "url": "http://primer3.ut.ee/", "citation": "https://dx.doi.org/10.1093/nar/gks596", "license": "", "publisher": "ELIXIR-EE", "operatingSystem": ["Linux", "Windows", "Mac"], "keywords": ["Probes and primers", "Web application"]}</a:t>
+            <a:t>{ </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>"@context": "http://schema.org",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  "@type": "SoftwareApplication",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  "name": "Primer3",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  "description": "The open-source software which is a widely used application for PCR primer design that includes more accurate thermodynamic models and the ability to use lowercase masked template sequences.",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  "softwareVersion": "1.0",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  "url": "http://primer3.ut.ee/",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  "citation": "https://dx.doi.org/10.1093/nar/gks596",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  "license": "",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  "publisher": "ELIXIR-EE",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  "operatingSystem": ["Linux", "Windows", "Mac"],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  "keywords": ["Probes and primers", "Web application"]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>}</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
@@ -635,7 +815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -868,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>

</xml_diff>